<commit_message>
Se agrega el scrap de Plumbersstock Auto_scrap_Plumbersstock.py.
</commit_message>
<xml_diff>
--- a/XX_Url/AmericanStandardUS.xlsx
+++ b/XX_Url/AmericanStandardUS.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/Pricing/Scrapping_git/XX_Url/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/Pricing/00_Sprint/00_Scrapping_code/XX_Url/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{ADD8D484-5C23-40E6-B751-62A63769F47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B0E4E69-0A11-4B3F-976A-7A3FF1B0F290}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{ADD8D484-5C23-40E6-B751-62A63769F47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32B4788A-AD6A-4A9D-8429-D05818BC2952}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="HomeDepot_URL" sheetId="2" r:id="rId1"/>
+    <sheet name="URL" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1141,7 +1141,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>